<commit_message>
Initial commit - Face Recognition Attendance System
</commit_message>
<xml_diff>
--- a/new_attendance.xlsx
+++ b/new_attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>2025-03-20</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2025-03-30</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,6 +461,7 @@
           <t>✅ 15:57</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -466,6 +472,24 @@
       <c r="B3" t="inlineStr">
         <is>
           <t>✅ 15:58</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>✅ 21:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hema</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>✅ 21:58</t>
         </is>
       </c>
     </row>

</xml_diff>